<commit_message>
Process config file is prepared
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BANCO\BamProcess\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\CinepolishArgentina\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C038D5B-2394-42AF-9905-706613D92CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -41,182 +42,79 @@
     <t>MaxRetryNumber</t>
   </si>
   <si>
-    <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
   </si>
   <si>
     <t>OrchestratorAssetFolder</t>
   </si>
   <si>
-    <t>BAM_URL</t>
+    <t>DirectorioClavesPath</t>
   </si>
   <si>
-    <t>01_LogFileInitialName</t>
+    <t>BlackListTrackingPath</t>
   </si>
   <si>
-    <t>01_BAM_URL</t>
+    <t>TRADPath</t>
   </si>
   <si>
-    <t>01_BAM_Credentials</t>
+    <t>InputFilePath</t>
   </si>
   <si>
-    <t>BamCred</t>
+    <t>FTPport</t>
   </si>
   <si>
-    <t>LogFileNameInit</t>
+    <t>FTPserver</t>
   </si>
   <si>
-    <t>DBColumns</t>
+    <t>FTPUser</t>
   </si>
   <si>
-    <t>01_BAM_DB_TableColumns</t>
+    <t>FTPPass</t>
   </si>
   <si>
-    <t>FTPFolderPath</t>
+    <t>in_BlackListSheetName</t>
   </si>
   <si>
-    <t>01_BAM_FTP_Path</t>
+    <t>in_TradSheetName</t>
   </si>
   <si>
-    <t>StandardColumns</t>
+    <t>Hoja 1</t>
   </si>
   <si>
-    <t>01_BAM_StandardTableColumns</t>
+    <t>Nft8}4zxb)RV</t>
   </si>
   <si>
-    <t>01_BAM_DB_TableName</t>
+    <t>ftp.tecnoyar.com</t>
   </si>
   <si>
-    <t>DBTableName</t>
+    <t>rpanotificaciones@tecnoyar.com</t>
   </si>
   <si>
-    <t>ErrorImageNameInit</t>
+    <t>TempSheetName</t>
   </si>
   <si>
-    <t>01_ErrorImageInitialName</t>
+    <t>GmailID</t>
   </si>
   <si>
-    <t>01_ExceptionMailID</t>
+    <t>GmailPass</t>
   </si>
   <si>
-    <t>ExceptionMailID</t>
+    <t>NO_SOCIOS_BD_Argentina__Semana_</t>
   </si>
   <si>
-    <t>01_BAM_SendFromEmail</t>
+    <t>notificacionesrpa.tecnoyar@gmail.com</t>
   </si>
   <si>
-    <t>SendMailFromCred</t>
+    <t>Rp4.C1n3p0l1s</t>
   </si>
   <si>
-    <t>01_SendEmailServer</t>
-  </si>
-  <si>
-    <t>SendEmailServer</t>
-  </si>
-  <si>
-    <t>01_SendEmailPort</t>
-  </si>
-  <si>
-    <t>SendEmailPort</t>
-  </si>
-  <si>
-    <t>BAM_DB_BankColHeader</t>
-  </si>
-  <si>
-    <t>01_BAM_DB_BankColHeader</t>
-  </si>
-  <si>
-    <t>01_BAM_DB_CUENTAColHeader</t>
-  </si>
-  <si>
-    <t>BAM_DB_CUENTAColHeader</t>
-  </si>
-  <si>
-    <t>01_BAM_DB_ID_BAM_ECColHeader</t>
-  </si>
-  <si>
-    <t>BAM_DB_ID_BAM_ECColHeader</t>
-  </si>
-  <si>
-    <t>01_BAM_DB_FetchAccountQuerry</t>
-  </si>
-  <si>
-    <t>BAM_DB_FetchAccountQuerry</t>
-  </si>
-  <si>
-    <t>01_BAM_DB_CommonColumns</t>
-  </si>
-  <si>
-    <t>BAM_DB_CommonColumns</t>
-  </si>
-  <si>
-    <t>BAM_FTP_Cred</t>
-  </si>
-  <si>
-    <t>01_BAM_FTP_Cred</t>
-  </si>
-  <si>
-    <t>01_BAM_FTP_Host</t>
-  </si>
-  <si>
-    <t>BAM_FTP_Host</t>
-  </si>
-  <si>
-    <t>BAM_FTP_Port</t>
-  </si>
-  <si>
-    <t>01_BAM_FTP_Port</t>
-  </si>
-  <si>
-    <t>01_BAM_DB_DataBaseCred</t>
-  </si>
-  <si>
-    <t>DBCred</t>
-  </si>
-  <si>
-    <t>BAM_DB_DataBaseNAME</t>
-  </si>
-  <si>
-    <t>01_BAM_DB_DataBaseNAME</t>
-  </si>
-  <si>
-    <t>BAM_DB_FECHA_CREACIONColHeader</t>
-  </si>
-  <si>
-    <t>01_BAM_DB_FECHA_CREACIONColHeader</t>
-  </si>
-  <si>
-    <t>BAM_DB_MONEDAColHeader</t>
-  </si>
-  <si>
-    <t>01_BAM_DB_MONEDAColHeader</t>
+    <t>TempBDPath</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18">
     <font>
       <sz val="11"/>
@@ -291,13 +189,6 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF4E5E65"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF4E5E65"/>
       <name val="Arial"/>
@@ -326,6 +217,12 @@
       <sz val="10"/>
       <color rgb="FF4E5E65"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -686,14 +583,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
@@ -737,26 +634,29 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="30">
-      <c r="A4" t="s">
-        <v>6</v>
+    <row r="4" spans="1:26">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1759,14 +1659,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z980"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
@@ -1816,49 +1716,37 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>17</v>
+      <c r="B4" s="18" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>32</v>
-      </c>
+      <c r="B5" s="16"/>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>49</v>
-      </c>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="B7" s="2"/>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>54</v>
-      </c>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="B8" s="12"/>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B10" s="12"/>
-    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2827,8 +2715,6 @@
     <row r="976" ht="14.25" customHeight="1"/>
     <row r="977" ht="14.25" customHeight="1"/>
     <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2837,14 +2723,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
@@ -2860,7 +2746,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2890,192 +2776,114 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="B2" s="5"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="B3" s="5"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="B4" s="6"/>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="B5" s="5"/>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>25</v>
-      </c>
+      <c r="B6" s="7"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>26</v>
+      <c r="B7" s="7">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>29</v>
+      <c r="B8" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>31</v>
+      <c r="A9" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" s="8" t="s">
-        <v>35</v>
+      <c r="A10" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>36</v>
-      </c>
+      <c r="A11" s="8"/>
+      <c r="B11" s="15"/>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="12"/>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" t="s">
-        <v>42</v>
-      </c>
+      <c r="A14" s="2"/>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>44</v>
-      </c>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>46</v>
-      </c>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
     </row>
-    <row r="17" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>50</v>
-      </c>
+    <row r="17" spans="2:3" ht="14.25" customHeight="1">
+      <c r="B17" s="13"/>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>53</v>
-      </c>
+    <row r="18" spans="2:3" ht="14.25" customHeight="1">
+      <c r="B18" s="14"/>
       <c r="C18" s="12"/>
     </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>57</v>
-      </c>
+    <row r="19" spans="2:3" ht="14.25" customHeight="1">
+      <c r="B19" s="17"/>
     </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="20" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="2:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -4046,7 +3854,10 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{FF7F0B36-CE90-4A91-B3A6-3587652CB510}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Partner and non partner process integrated
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\CinepolishArgentina\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C038D5B-2394-42AF-9905-706613D92CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224B0270-2B73-4300-812F-EDEE5248C107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>TRADPath</t>
-  </si>
-  <si>
-    <t>InputFilePath</t>
   </si>
   <si>
     <t>FTPport</t>
@@ -108,14 +105,41 @@
     <t>Rp4.C1n3p0l1s</t>
   </si>
   <si>
-    <t>TempBDPath</t>
+    <t>PartnerTempBDPath</t>
+  </si>
+  <si>
+    <t>NonPartnerTempBDPath</t>
+  </si>
+  <si>
+    <t>InputnonPartnerFilePath</t>
+  </si>
+  <si>
+    <t>InputPartnerFilePath</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/30 Envio Semana 30/Argentina/Base de Datos/No Socios</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/30 Envio Semana 30/Argentina/Base de Datos/Socios</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/30 Envio Semana 30/Argentina/Tradicional/No Socios</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/30 Envio Semana 30/Argentina/Tradicional/Socios</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/1 Directorio</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/30 Envio Semana 30/Argentina/Base de Datos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -137,12 +161,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF485056"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -225,6 +243,18 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -246,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -257,7 +287,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -269,7 +298,36 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,14 +644,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="2" max="2" width="68" style="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -602,7 +660,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -634,41 +692,118 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>17</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="21" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>24</v>
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="17">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -1653,8 +1788,11 @@
     <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B13" r:id="rId1" xr:uid="{FF7F0B36-CE90-4A91-B3A6-3587652CB510}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1662,8 +1800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1721,29 +1859,29 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B5" s="16"/>
+      <c r="B5" s="14"/>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B8" s="12"/>
+      <c r="B8" s="10"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2724,10 +2862,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2774,116 +2912,64 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="5"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="C11" s="10"/>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="5"/>
-    </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="6"/>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="5"/>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="7"/>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="7">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="12"/>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="15"/>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="12"/>
-    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="13"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="2"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
+      <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="2:3" ht="14.25" customHeight="1">
-      <c r="B17" s="13"/>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
     </row>
-    <row r="18" spans="2:3" ht="14.25" customHeight="1">
-      <c r="B18" s="14"/>
-      <c r="C18" s="12"/>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
     </row>
-    <row r="19" spans="2:3" ht="14.25" customHeight="1">
-      <c r="B19" s="17"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="B19" s="11"/>
     </row>
-    <row r="20" spans="2:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="2:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="2:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="2:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="2:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="2:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="2:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="2:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="2:3" ht="14.25" customHeight="1"/>
-    <row r="29" spans="2:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="2:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="2:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="B20" s="12"/>
+      <c r="C20" s="10"/>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="B21" s="15"/>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -3852,12 +3938,11 @@
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
+    <row r="1002" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" xr:uid="{FF7F0B36-CE90-4A91-B3A6-3587652CB510}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
input file path implimented
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\CinepolishArgentina\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224B0270-2B73-4300-812F-EDEE5248C107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D0A29F-B4DA-47B7-BCC7-6D91C5A3DDA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -133,6 +133,15 @@
   </si>
   <si>
     <t>/Planeacion/0.Envios TS 2021/30 Envio Semana 30/Argentina/Base de Datos</t>
+  </si>
+  <si>
+    <t>InputFilePath</t>
+  </si>
+  <si>
+    <t>input file path for partner file</t>
+  </si>
+  <si>
+    <t>input file path for non partner file</t>
   </si>
 </sst>
 </file>
@@ -645,7 +654,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -763,6 +772,9 @@
       <c r="B10" s="17" t="s">
         <v>32</v>
       </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
@@ -771,6 +783,9 @@
       <c r="B11" s="24" t="s">
         <v>31</v>
       </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
@@ -804,7 +819,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
testing done for the artifect.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\CinepolishArgentina\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\CinepolisArgentina\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6A341D-3435-4E0E-85AA-88E9C0A740E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DF8019-149B-455A-BAF0-014A015AB6E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -135,13 +135,16 @@
     <t>/Planeacion/0.Envios TS 2021/30 Envio Semana 30/Argentina/Base de Datos</t>
   </si>
   <si>
-    <t>InputFilePath</t>
-  </si>
-  <si>
     <t>input file path for partner file</t>
   </si>
   <si>
     <t>input file path for non partner file</t>
+  </si>
+  <si>
+    <t>TempPartnerSheetName</t>
+  </si>
+  <si>
+    <t>SOCIOS_BD_Argentina_Semana_Sema</t>
   </si>
 </sst>
 </file>
@@ -651,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -773,7 +776,7 @@
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -784,7 +787,7 @@
         <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -821,7 +824,10 @@
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1"/>
@@ -1804,7 +1810,6 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>

</xml_diff>

<commit_message>
testing done for argentina
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\CinepolisArgentina\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D3E2C0-AAB8-4386-A501-71CF81C02058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365FB8D2-D880-4564-B935-ABCCF47583DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1545" yWindow="0" windowWidth="16140" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -117,9 +117,6 @@
     <t>InputPartnerFilePath</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS 2021/1 Directorio</t>
-  </si>
-  <si>
     <t>TempPartnerSheetName</t>
   </si>
   <si>
@@ -144,29 +141,32 @@
     <t>Archivo de entrada para no socios</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS 2021/36 Envio Semana 36/ARGENTINA/Base de Datos</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/36 Envio Semana 36/ARGENTINA/Tradicional/No Socio</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/36 Envio Semana 36/ARGENTINA/Tradicional/Socios</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/36 Envio Semana 36/ARGENTINA/Base de Datos/SOCIOS</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/36 Envio Semana 36/ARGENTINA/Base de Datos/NO_SOCIO</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/36 Envio Semana 36/ARGENTINA/Base de Datos/Exportadas</t>
+    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/ARGENTINA/Base de Datos</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/ARGENTINA/Base de Datos/NO_SOCIO</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/ARGENTINA/Base de Datos/SOCIOS</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/1 Directorio</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/ARGENTINA/Tradicional/Socios</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/ARGENTINA/Tradicional/No Socio</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/ARGENTINA/Base de Datos/Exportadas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -271,12 +271,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -303,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -325,7 +319,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -340,13 +334,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -672,7 +663,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -748,10 +739,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -759,10 +750,10 @@
         <v>27</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -770,10 +761,10 @@
         <v>28</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -781,10 +772,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -799,22 +790,22 @@
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>43</v>
+      <c r="B10" s="22" t="s">
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>44</v>
+      <c r="B11" s="22" t="s">
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -829,7 +820,7 @@
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="24" t="s">
         <v>19</v>
       </c>
     </row>
@@ -837,7 +828,7 @@
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="25" t="s">
         <v>20</v>
       </c>
     </row>
@@ -845,16 +836,16 @@
       <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="25" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="21" t="s">
         <v>32</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
blacklist checked and updated
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\CinepolisArgentina\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6FD203-9C6F-4A0E-A6AB-99A8A7B2AAA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5416A4-18A2-4BD9-AB92-D90F5500841A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="495" windowWidth="16140" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -144,27 +144,9 @@
     <t>/Planeacion/0.Envios TS/1 Directorio</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/ARGENTINA/Base de Datos/NO_SOCIO</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/ARGENTINA/Base de Datos/SOCIOS</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/ARGENTINA/Base de Datos/Exportadas</t>
-  </si>
-  <si>
     <t>Archivos exportados</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/ARGENTINA/Tradicional/No Socio</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/ARGENTINA/Tradicional/Socios</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/ARGENTINA/Base de Datos</t>
-  </si>
-  <si>
     <t>CorrectnameFilePath</t>
   </si>
   <si>
@@ -184,6 +166,27 @@
   </si>
   <si>
     <t>Hoja</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/ARGENTINA/Base de Datos</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/ARGENTINA/Tradicional/Socios</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/ARGENTINA/Tradicional/No Socio</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/ARGENTINA/Base de Datos/Exportadas</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/ARGENTINA/Base de Datos/SOCIOS</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/ARGENTINA/Base de Datos/NO_SOCIO</t>
+  </si>
+  <si>
+    <t>Black List</t>
   </si>
 </sst>
 </file>
@@ -690,7 +693,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -740,7 +743,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -766,7 +769,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
         <v>33</v>
@@ -777,7 +780,7 @@
         <v>27</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
@@ -788,7 +791,7 @@
         <v>28</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
         <v>35</v>
@@ -810,10 +813,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -821,7 +824,7 @@
         <v>30</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
         <v>37</v>
@@ -832,7 +835,7 @@
         <v>29</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
@@ -881,18 +884,18 @@
     <row r="17" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" s="26" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" s="26" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
@@ -1964,24 +1967,24 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="26" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B6" s="27">
-        <v>44599</v>
+        <v>44613</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="26" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B7" s="27">
-        <v>44605</v>
+        <v>44619</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>